<commit_message>
Module deleted for moving to other folder.
</commit_message>
<xml_diff>
--- a/Lia/Lia.xlsx
+++ b/Lia/Lia.xlsx
@@ -4,19 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="8385" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Частоты" sheetId="2" r:id="rId2"/>
     <sheet name="816" sheetId="3" r:id="rId3"/>
+    <sheet name="Tirno BOM" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tirno BOM'!$A$1:$C$1</definedName>
+    <definedName name="tirno" localSheetId="3">'Tirno BOM'!$A$1:$C$78</definedName>
+  </definedNames>
   <calcPr calcId="144315"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="tirno" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="D:\Nute\Lia\Tirno\Hardware\tirno.txt" thousands=" " tab="0" semicolon="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="157">
   <si>
     <t>MHz</t>
   </si>
@@ -142,6 +161,351 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>footprint</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C51</t>
+  </si>
+  <si>
+    <t>C81</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>C111</t>
+  </si>
+  <si>
+    <t>2p2</t>
+  </si>
+  <si>
+    <t>C121</t>
+  </si>
+  <si>
+    <t>1p</t>
+  </si>
+  <si>
+    <t>C122</t>
+  </si>
+  <si>
+    <t>1p5</t>
+  </si>
+  <si>
+    <t>C123</t>
+  </si>
+  <si>
+    <t>3p3</t>
+  </si>
+  <si>
+    <t>C124</t>
+  </si>
+  <si>
+    <t>100p</t>
+  </si>
+  <si>
+    <t>C125</t>
+  </si>
+  <si>
+    <t>12p</t>
+  </si>
+  <si>
+    <t>C131</t>
+  </si>
+  <si>
+    <t>C141</t>
+  </si>
+  <si>
+    <t>C151</t>
+  </si>
+  <si>
+    <t>220p</t>
+  </si>
+  <si>
+    <t>C181</t>
+  </si>
+  <si>
+    <t>C1231</t>
+  </si>
+  <si>
+    <t>6p8</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D_SHOTTKY</t>
+  </si>
+  <si>
+    <t>DA1</t>
+  </si>
+  <si>
+    <t>LM2703</t>
+  </si>
+  <si>
+    <t>DA2</t>
+  </si>
+  <si>
+    <t>AAT3221</t>
+  </si>
+  <si>
+    <t>DD1</t>
+  </si>
+  <si>
+    <t>ATMEGA324</t>
+  </si>
+  <si>
+    <t>DD2</t>
+  </si>
+  <si>
+    <t>CC1101</t>
+  </si>
+  <si>
+    <t>DD3</t>
+  </si>
+  <si>
+    <t>FT232R</t>
+  </si>
+  <si>
+    <t>HOLE1</t>
+  </si>
+  <si>
+    <t>HOLE_METALLED</t>
+  </si>
+  <si>
+    <t>HOLE2</t>
+  </si>
+  <si>
+    <t>HOLE3</t>
+  </si>
+  <si>
+    <t>HOLE4</t>
+  </si>
+  <si>
+    <t>1.8uH</t>
+  </si>
+  <si>
+    <t>L121</t>
+  </si>
+  <si>
+    <t>12nH</t>
+  </si>
+  <si>
+    <t>L122</t>
+  </si>
+  <si>
+    <t>18nH</t>
+  </si>
+  <si>
+    <t>L123</t>
+  </si>
+  <si>
+    <t>L124</t>
+  </si>
+  <si>
+    <t>L131</t>
+  </si>
+  <si>
+    <t>L132</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>NOKIA1100</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>IRLML6302</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R171</t>
+  </si>
+  <si>
+    <t>56k</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>PUSHBUTTON</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>TP1</t>
+  </si>
+  <si>
+    <t>TESTPOINT</t>
+  </si>
+  <si>
+    <t>TP2</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>TP4</t>
+  </si>
+  <si>
+    <t>TP5</t>
+  </si>
+  <si>
+    <t>TP6</t>
+  </si>
+  <si>
+    <t>TP7</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>TP9</t>
+  </si>
+  <si>
+    <t>TP10</t>
+  </si>
+  <si>
+    <t>TP11</t>
+  </si>
+  <si>
+    <t>XL1</t>
+  </si>
+  <si>
+    <t>PWRCONN</t>
+  </si>
+  <si>
+    <t>XL3</t>
+  </si>
+  <si>
+    <t>CONN_2</t>
+  </si>
+  <si>
+    <t>XL4</t>
+  </si>
+  <si>
+    <t>ATMEL_JTAG</t>
+  </si>
+  <si>
+    <t>XL5</t>
+  </si>
+  <si>
+    <t>USB_MINI_B</t>
+  </si>
+  <si>
+    <t>XL6</t>
+  </si>
+  <si>
+    <t>SMA_L</t>
+  </si>
+  <si>
+    <t>XL7</t>
+  </si>
+  <si>
+    <t>CONN_3</t>
+  </si>
+  <si>
+    <t>XTAL1</t>
+  </si>
+  <si>
+    <t>26MHz</t>
   </si>
 </sst>
 </file>
@@ -229,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -267,6 +631,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -275,7 +648,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -284,6 +657,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -300,6 +676,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tirno" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1124,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1159,4 +1539,653 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>